<commit_message>
Added example of red circle detection.
</commit_message>
<xml_diff>
--- a/RoadSigns.xlsx
+++ b/RoadSigns.xlsx
@@ -1351,7 +1351,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -3340,7 +3340,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -4190,7 +4190,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -4632,7 +4632,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -4972,7 +4972,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -5125,7 +5125,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5720,7 +5720,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5975,7 +5975,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -7403,7 +7403,7 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -7539,7 +7539,7 @@
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -7726,7 +7726,7 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -7930,7 +7930,7 @@
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -8015,7 +8015,7 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -8032,7 +8032,7 @@
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -8270,7 +8270,7 @@
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -8355,7 +8355,7 @@
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -8627,7 +8627,7 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -8746,7 +8746,7 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -8780,7 +8780,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -8984,7 +8984,7 @@
       </c>
       <c r="C504" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -9001,7 +9001,7 @@
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -9120,7 +9120,7 @@
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -9188,7 +9188,7 @@
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -9324,7 +9324,7 @@
       </c>
       <c r="C524" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Basic Stop Algorithm add
</commit_message>
<xml_diff>
--- a/RoadSigns.xlsx
+++ b/RoadSigns.xlsx
@@ -739,7 +739,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -3323,7 +3323,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -3777,12 +3777,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -3918,7 +3918,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -3964,12 +3964,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4372,12 +4372,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -4542,12 +4542,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -4712,12 +4712,12 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -4899,12 +4899,12 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5035,12 +5035,12 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5108,7 +5108,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5205,12 +5205,12 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5278,7 +5278,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5295,7 +5295,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5392,12 +5392,12 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5409,12 +5409,12 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5426,12 +5426,12 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5443,12 +5443,12 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5460,12 +5460,12 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5477,12 +5477,12 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5494,12 +5494,12 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5511,7 +5511,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -5562,12 +5562,12 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5732,12 +5732,12 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5783,7 +5783,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -5907,7 +5907,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -5958,7 +5958,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -5970,12 +5970,12 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -6055,7 +6055,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -6072,7 +6072,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -6094,7 +6094,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -6140,12 +6140,12 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -6310,12 +6310,12 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -6582,12 +6582,12 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -6706,7 +6706,7 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -6888,12 +6888,12 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -6944,7 +6944,7 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7024,7 +7024,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
@@ -7211,12 +7211,12 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7398,12 +7398,12 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7539,7 +7539,7 @@
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7568,12 +7568,12 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7590,7 +7590,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7607,7 +7607,7 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7692,7 +7692,7 @@
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -7891,12 +7891,12 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8078,12 +8078,12 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8265,12 +8265,12 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8384,12 +8384,12 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8406,7 +8406,7 @@
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8423,7 +8423,7 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8440,7 +8440,7 @@
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8474,7 +8474,7 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8537,12 +8537,12 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8644,7 +8644,7 @@
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -8661,7 +8661,7 @@
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -8724,12 +8724,12 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -8746,7 +8746,7 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>speedlimit</t>
         </is>
       </c>
     </row>
@@ -8911,12 +8911,12 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9268,12 +9268,12 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C521" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C524" t="inlineStr">
@@ -9336,7 +9336,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C525" t="inlineStr">
@@ -9353,7 +9353,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C526" t="inlineStr">
@@ -9370,7 +9370,7 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C527" t="inlineStr">
@@ -9387,7 +9387,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C528" t="inlineStr">
@@ -9404,7 +9404,7 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C529" t="inlineStr">
@@ -9421,12 +9421,12 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C530" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9438,12 +9438,12 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C531" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9455,12 +9455,12 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C532" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9472,12 +9472,12 @@
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C533" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9489,12 +9489,12 @@
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C534" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9506,12 +9506,12 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C535" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>
@@ -9523,12 +9523,12 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>stop</t>
         </is>
       </c>
       <c r="C536" t="inlineStr">
         <is>
-          <t>speedlimit</t>
+          <t>stop</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improvement with dilates to blue squares
</commit_message>
<xml_diff>
--- a/RoadSigns.xlsx
+++ b/RoadSigns.xlsx
@@ -875,7 +875,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -960,7 +960,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -994,7 +994,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -4156,7 +4156,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -4411,7 +4411,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -5312,7 +5312,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -5771,7 +5771,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -5788,7 +5788,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -6128,7 +6128,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -6485,7 +6485,7 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -6825,7 +6825,7 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -7250,7 +7250,7 @@
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -7267,7 +7267,7 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -7335,7 +7335,7 @@
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>crosswalk</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -7386,7 +7386,7 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -7403,7 +7403,7 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -8542,7 +8542,7 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -8559,7 +8559,7 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>crosswalk</t>
+          <t>other</t>
         </is>
       </c>
     </row>
@@ -8899,7 +8899,7 @@
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9256,7 +9256,7 @@
       </c>
       <c r="C520" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9460,7 +9460,7 @@
       </c>
       <c r="C532" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9834,7 +9834,7 @@
       </c>
       <c r="C554" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9868,7 +9868,7 @@
       </c>
       <c r="C556" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9885,7 +9885,7 @@
       </c>
       <c r="C557" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9902,7 +9902,7 @@
       </c>
       <c r="C558" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9919,7 +9919,7 @@
       </c>
       <c r="C559" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9936,7 +9936,7 @@
       </c>
       <c r="C560" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -9953,7 +9953,7 @@
       </c>
       <c r="C561" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -10055,7 +10055,7 @@
       </c>
       <c r="C567" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -10242,7 +10242,7 @@
       </c>
       <c r="C578" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>
@@ -10259,7 +10259,7 @@
       </c>
       <c r="C579" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>crosswalk</t>
         </is>
       </c>
     </row>

</xml_diff>